<commit_message>
'scenTable.xlsx' converted in .csv
</commit_message>
<xml_diff>
--- a/docs/scenTable.xlsx
+++ b/docs/scenTable.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="592" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="594" uniqueCount="69">
   <si>
     <t xml:space="preserve">id</t>
   </si>
@@ -264,11 +264,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
     <numFmt numFmtId="166" formatCode="YYYY/MM/DD"/>
-    <numFmt numFmtId="167" formatCode="YYYY/MM/DD"/>
   </numFmts>
   <fonts count="9">
     <font>
@@ -506,7 +505,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -518,11 +517,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1651,9 +1650,7 @@
   <dimension ref="A1:M46"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="555" topLeftCell="A13" activePane="bottomLeft" state="split"/>
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="L20" activeCellId="0" sqref="L20"/>
+      <selection pane="topLeft" activeCell="H3" activeCellId="0" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1705,7 +1702,7 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="24" t="s">
         <v>14</v>
       </c>
       <c r="B2" s="7" t="s">
@@ -1746,7 +1743,7 @@
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="6" t="s">
+      <c r="A3" s="24" t="s">
         <v>21</v>
       </c>
       <c r="B3" s="7" t="s">
@@ -1787,7 +1784,7 @@
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="6" t="s">
+      <c r="A4" s="24" t="s">
         <v>24</v>
       </c>
       <c r="B4" s="7" t="s">
@@ -1828,7 +1825,7 @@
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="6" t="s">
+      <c r="A5" s="24" t="s">
         <v>26</v>
       </c>
       <c r="B5" s="7" t="s">
@@ -1869,7 +1866,7 @@
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="6" t="s">
+      <c r="A6" s="24" t="s">
         <v>29</v>
       </c>
       <c r="B6" s="7" t="s">
@@ -1910,7 +1907,7 @@
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="6" t="s">
+      <c r="A7" s="24" t="s">
         <v>32</v>
       </c>
       <c r="B7" s="7" t="s">
@@ -1951,7 +1948,7 @@
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="6" t="s">
+      <c r="A8" s="24" t="s">
         <v>35</v>
       </c>
       <c r="B8" s="7" t="s">
@@ -1992,7 +1989,7 @@
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="6" t="s">
+      <c r="A9" s="24" t="s">
         <v>37</v>
       </c>
       <c r="B9" s="7" t="s">
@@ -2033,7 +2030,7 @@
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="6" t="s">
+      <c r="A10" s="24" t="s">
         <v>39</v>
       </c>
       <c r="B10" s="7" t="s">
@@ -2074,7 +2071,7 @@
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="6" t="s">
+      <c r="A11" s="24" t="s">
         <v>41</v>
       </c>
       <c r="B11" s="7" t="s">
@@ -2115,7 +2112,7 @@
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="6" t="s">
+      <c r="A12" s="24" t="s">
         <v>43</v>
       </c>
       <c r="B12" s="7" t="s">
@@ -2156,7 +2153,7 @@
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="20" t="s">
+      <c r="A13" s="24" t="s">
         <v>45</v>
       </c>
       <c r="B13" s="7" t="s">
@@ -2397,12 +2394,12 @@
       <c r="L18" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="M18" s="24" t="n">
-        <v>43932</v>
+      <c r="M18" s="0" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="6" t="s">
+      <c r="A19" s="24" t="s">
         <v>58</v>
       </c>
       <c r="B19" s="7" t="s">
@@ -2438,9 +2435,12 @@
       <c r="L19" s="11" t="s">
         <v>17</v>
       </c>
+      <c r="M19" s="0" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="6" t="s">
+      <c r="A20" s="24" t="s">
         <v>59</v>
       </c>
       <c r="B20" s="7" t="s">

</xml_diff>

<commit_message>
Analysis completed - submitted ms
</commit_message>
<xml_diff>
--- a/docs/scenTable.xlsx
+++ b/docs/scenTable.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="594" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="608" uniqueCount="71">
   <si>
     <t xml:space="preserve">id</t>
   </si>
@@ -245,6 +245,12 @@
     <t xml:space="preserve">Var. Reten &amp; salvage logging w. post-fire planting (Jack Pine), no access constrains</t>
   </si>
   <si>
+    <t xml:space="preserve">simID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">id_ms</t>
+  </si>
+  <si>
     <t xml:space="preserve">sim. Status</t>
   </si>
   <si>
@@ -267,7 +273,7 @@
   <numFmts count="3">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
-    <numFmt numFmtId="166" formatCode="YYYY/MM/DD"/>
+    <numFmt numFmtId="166" formatCode="yyyy/mm/dd"/>
   </numFmts>
   <fonts count="9">
     <font>
@@ -610,17 +616,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:N23"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="N23" activeCellId="0" sqref="N23"/>
+      <selection pane="topLeft" activeCell="A9" activeCellId="0" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="8.89"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="8.89"/>
@@ -628,9 +634,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="4" style="2" width="8.89"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="8" style="2" width="15.68"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="22.36"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="22.36"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="16" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1643,80 +1647,82 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:M46"/>
+  <dimension ref="A1:N46"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H3" activeCellId="0" sqref="H3"/>
+      <selection pane="topLeft" activeCell="B16" activeCellId="0" sqref="B16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="63.26"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="4" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="63.26"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="12.64"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="21" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="22" t="s">
+        <v>64</v>
+      </c>
+      <c r="B1" s="21" t="s">
+        <v>65</v>
+      </c>
+      <c r="C1" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="22" t="s">
+      <c r="D1" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="22" t="s">
+      <c r="E1" s="22" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="22" t="s">
+      <c r="F1" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="22" t="s">
+      <c r="G1" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="22" t="s">
+      <c r="H1" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="22" t="s">
+      <c r="I1" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="22" t="s">
+      <c r="J1" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="22" t="s">
+      <c r="K1" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="22" t="s">
+      <c r="L1" s="22" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="22" t="s">
+      <c r="M1" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="23" t="s">
-        <v>64</v>
+      <c r="N1" s="23" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="B2" s="7" t="s">
-        <v>15</v>
+      <c r="B2" s="24" t="s">
+        <v>14</v>
       </c>
       <c r="C2" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="D2" s="7" t="n">
+      <c r="E2" s="7" t="n">
         <v>0</v>
       </c>
-      <c r="E2" s="8" t="s">
-        <v>17</v>
-      </c>
       <c r="F2" s="8" t="s">
         <v>17</v>
       </c>
@@ -1726,8 +1732,8 @@
       <c r="H2" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="I2" s="7" t="s">
-        <v>18</v>
+      <c r="I2" s="8" t="s">
+        <v>17</v>
       </c>
       <c r="J2" s="7" t="s">
         <v>18</v>
@@ -1738,7 +1744,10 @@
       <c r="L2" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="M2" s="9" t="s">
+      <c r="M2" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="N2" s="9" t="s">
         <v>19</v>
       </c>
     </row>
@@ -1746,40 +1755,41 @@
       <c r="A3" s="24" t="s">
         <v>21</v>
       </c>
-      <c r="B3" s="7" t="s">
-        <v>15</v>
-      </c>
+      <c r="B3" s="24"/>
       <c r="C3" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="D3" s="7" t="n">
-        <v>0.0062</v>
-      </c>
-      <c r="E3" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="F3" s="8" t="s">
-        <v>17</v>
+      <c r="E3" s="7" t="n">
+        <v>0.0062</v>
+      </c>
+      <c r="F3" s="10" t="s">
+        <v>23</v>
       </c>
       <c r="G3" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="H3" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="I3" s="2" t="s">
-        <v>18</v>
+      <c r="H3" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="I3" s="11" t="s">
+        <v>17</v>
       </c>
       <c r="J3" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="K3" s="7" t="s">
+      <c r="K3" s="2" t="s">
         <v>18</v>
       </c>
       <c r="L3" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="M3" s="12" t="s">
+      <c r="M3" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="N3" s="12" t="s">
         <v>19</v>
       </c>
     </row>
@@ -1787,40 +1797,41 @@
       <c r="A4" s="24" t="s">
         <v>24</v>
       </c>
-      <c r="B4" s="7" t="s">
-        <v>15</v>
-      </c>
+      <c r="B4" s="24"/>
       <c r="C4" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="D4" s="7" t="n">
-        <v>0.0062</v>
-      </c>
-      <c r="E4" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="F4" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="G4" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="H4" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="I4" s="2" t="s">
-        <v>18</v>
+      <c r="E4" s="7" t="n">
+        <v>0.0062</v>
+      </c>
+      <c r="F4" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="G4" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="H4" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="I4" s="11" t="s">
+        <v>17</v>
       </c>
       <c r="J4" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="K4" s="7" t="s">
+      <c r="K4" s="2" t="s">
         <v>18</v>
       </c>
       <c r="L4" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="M4" s="9" t="s">
+      <c r="M4" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="N4" s="9" t="s">
         <v>19</v>
       </c>
     </row>
@@ -1828,40 +1839,41 @@
       <c r="A5" s="24" t="s">
         <v>26</v>
       </c>
-      <c r="B5" s="7" t="s">
-        <v>15</v>
-      </c>
+      <c r="B5" s="24"/>
       <c r="C5" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="D5" s="7" t="n">
-        <v>0.0062</v>
-      </c>
-      <c r="E5" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="F5" s="8" t="s">
-        <v>17</v>
+      <c r="E5" s="7" t="n">
+        <v>0.0062</v>
+      </c>
+      <c r="F5" s="10" t="s">
+        <v>23</v>
       </c>
       <c r="G5" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="H5" s="13" t="s">
-        <v>23</v>
-      </c>
-      <c r="I5" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="J5" s="14" t="s">
+      <c r="H5" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="I5" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="J5" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="K5" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="K5" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="L5" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="M5" s="9" t="s">
+      <c r="L5" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="M5" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="N5" s="9" t="s">
         <v>19</v>
       </c>
     </row>
@@ -1869,40 +1881,41 @@
       <c r="A6" s="24" t="s">
         <v>29</v>
       </c>
-      <c r="B6" s="7" t="s">
-        <v>15</v>
-      </c>
+      <c r="B6" s="24"/>
       <c r="C6" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="D6" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="D6" s="7" t="n">
-        <v>0.0062</v>
-      </c>
-      <c r="E6" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="F6" s="8" t="s">
-        <v>17</v>
+      <c r="E6" s="7" t="n">
+        <v>0.0062</v>
+      </c>
+      <c r="F6" s="10" t="s">
+        <v>23</v>
       </c>
       <c r="G6" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="H6" s="13" t="s">
-        <v>23</v>
-      </c>
-      <c r="I6" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="J6" s="15" t="s">
+      <c r="H6" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="I6" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="J6" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="K6" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="K6" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="L6" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="M6" s="9" t="s">
+      <c r="L6" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="M6" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="N6" s="9" t="s">
         <v>19</v>
       </c>
     </row>
@@ -1910,40 +1923,43 @@
       <c r="A7" s="24" t="s">
         <v>32</v>
       </c>
-      <c r="B7" s="7" t="s">
-        <v>15</v>
+      <c r="B7" s="24" t="s">
+        <v>26</v>
       </c>
       <c r="C7" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="D7" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="D7" s="7" t="n">
-        <v>0.0062</v>
-      </c>
-      <c r="E7" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="F7" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="G7" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="H7" s="13" t="s">
+      <c r="E7" s="7" t="n">
+        <v>0.0062</v>
+      </c>
+      <c r="F7" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="G7" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="H7" s="10" t="s">
         <v>23</v>
       </c>
       <c r="I7" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="J7" s="14" t="s">
+      <c r="J7" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="K7" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="K7" s="16" t="s">
+      <c r="L7" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="L7" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="M7" s="9" t="s">
+      <c r="M7" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="N7" s="9" t="s">
         <v>19</v>
       </c>
     </row>
@@ -1951,40 +1967,43 @@
       <c r="A8" s="24" t="s">
         <v>35</v>
       </c>
-      <c r="B8" s="7" t="s">
-        <v>15</v>
+      <c r="B8" s="24" t="s">
+        <v>29</v>
       </c>
       <c r="C8" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="D8" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="D8" s="7" t="n">
-        <v>0.0062</v>
-      </c>
-      <c r="E8" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="F8" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="G8" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="H8" s="13" t="s">
+      <c r="E8" s="7" t="n">
+        <v>0.0062</v>
+      </c>
+      <c r="F8" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="G8" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="H8" s="10" t="s">
         <v>23</v>
       </c>
       <c r="I8" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="J8" s="15" t="s">
+      <c r="J8" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="K8" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="K8" s="18" t="s">
+      <c r="L8" s="18" t="s">
         <v>31</v>
       </c>
-      <c r="L8" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="M8" s="9" t="s">
+      <c r="M8" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="N8" s="9" t="s">
         <v>19</v>
       </c>
     </row>
@@ -1992,40 +2011,43 @@
       <c r="A9" s="24" t="s">
         <v>37</v>
       </c>
-      <c r="B9" s="7" t="s">
-        <v>15</v>
+      <c r="B9" s="24" t="s">
+        <v>32</v>
       </c>
       <c r="C9" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="D9" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="D9" s="7" t="n">
-        <v>0.0062</v>
-      </c>
-      <c r="E9" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="F9" s="10" t="s">
-        <v>23</v>
+      <c r="E9" s="7" t="n">
+        <v>0.0062</v>
+      </c>
+      <c r="F9" s="8" t="s">
+        <v>17</v>
       </c>
       <c r="G9" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="H9" s="13" t="s">
+      <c r="H9" s="10" t="s">
         <v>23</v>
       </c>
       <c r="I9" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="J9" s="14" t="s">
+      <c r="J9" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="K9" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="K9" s="16" t="s">
+      <c r="L9" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="L9" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="M9" s="9" t="s">
+      <c r="M9" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="N9" s="9" t="s">
         <v>19</v>
       </c>
     </row>
@@ -2033,40 +2055,43 @@
       <c r="A10" s="24" t="s">
         <v>39</v>
       </c>
-      <c r="B10" s="7" t="s">
-        <v>15</v>
+      <c r="B10" s="24" t="s">
+        <v>35</v>
       </c>
       <c r="C10" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="D10" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="D10" s="7" t="n">
-        <v>0.0062</v>
-      </c>
-      <c r="E10" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="F10" s="10" t="s">
-        <v>23</v>
+      <c r="E10" s="7" t="n">
+        <v>0.0062</v>
+      </c>
+      <c r="F10" s="8" t="s">
+        <v>17</v>
       </c>
       <c r="G10" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="H10" s="13" t="s">
+      <c r="H10" s="10" t="s">
         <v>23</v>
       </c>
       <c r="I10" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="J10" s="15" t="s">
+      <c r="J10" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="K10" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="K10" s="18" t="s">
+      <c r="L10" s="18" t="s">
         <v>31</v>
       </c>
-      <c r="L10" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="M10" s="9" t="s">
+      <c r="M10" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="N10" s="9" t="s">
         <v>19</v>
       </c>
     </row>
@@ -2074,40 +2099,43 @@
       <c r="A11" s="24" t="s">
         <v>41</v>
       </c>
-      <c r="B11" s="7" t="s">
+      <c r="B11" s="24" t="s">
+        <v>41</v>
+      </c>
+      <c r="C11" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="C11" s="7" t="s">
+      <c r="D11" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="D11" s="7" t="n">
+      <c r="E11" s="7" t="n">
         <v>0</v>
       </c>
-      <c r="E11" s="8" t="s">
-        <v>17</v>
-      </c>
       <c r="F11" s="8" t="s">
         <v>17</v>
       </c>
       <c r="G11" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="H11" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="I11" s="2" t="s">
-        <v>18</v>
+      <c r="H11" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="I11" s="11" t="s">
+        <v>17</v>
       </c>
       <c r="J11" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="K11" s="7" t="s">
+      <c r="K11" s="2" t="s">
         <v>18</v>
       </c>
       <c r="L11" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="M11" s="0" t="s">
+      <c r="M11" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="N11" s="0" t="s">
         <v>19</v>
       </c>
     </row>
@@ -2115,40 +2143,43 @@
       <c r="A12" s="24" t="s">
         <v>43</v>
       </c>
-      <c r="B12" s="7" t="s">
+      <c r="B12" s="24" t="s">
+        <v>45</v>
+      </c>
+      <c r="C12" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="C12" s="7" t="s">
+      <c r="D12" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="D12" s="7" t="n">
-        <v>0.0062</v>
-      </c>
-      <c r="E12" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="F12" s="10" t="s">
-        <v>23</v>
+      <c r="E12" s="7" t="n">
+        <v>0.0062</v>
+      </c>
+      <c r="F12" s="8" t="s">
+        <v>17</v>
       </c>
       <c r="G12" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="H12" s="13" t="s">
+      <c r="H12" s="10" t="s">
         <v>23</v>
       </c>
       <c r="I12" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="J12" s="14" t="s">
+      <c r="J12" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="K12" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="K12" s="16" t="s">
+      <c r="L12" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="L12" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="M12" s="0" t="s">
+      <c r="M12" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="N12" s="0" t="s">
         <v>19</v>
       </c>
     </row>
@@ -2156,20 +2187,20 @@
       <c r="A13" s="24" t="s">
         <v>45</v>
       </c>
-      <c r="B13" s="7" t="s">
+      <c r="B13" s="24" t="s">
+        <v>47</v>
+      </c>
+      <c r="C13" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="C13" s="7" t="s">
+      <c r="D13" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="D13" s="7" t="n">
-        <v>0.0062</v>
-      </c>
-      <c r="E13" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="F13" s="10" t="s">
-        <v>23</v>
+      <c r="E13" s="7" t="n">
+        <v>0.0062</v>
+      </c>
+      <c r="F13" s="8" t="s">
+        <v>17</v>
       </c>
       <c r="G13" s="10" t="s">
         <v>23</v>
@@ -2180,16 +2211,19 @@
       <c r="I13" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="J13" s="18" t="s">
-        <v>31</v>
+      <c r="J13" s="10" t="s">
+        <v>23</v>
       </c>
       <c r="K13" s="18" t="s">
         <v>31</v>
       </c>
-      <c r="L13" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="M13" s="0" t="s">
+      <c r="L13" s="18" t="s">
+        <v>31</v>
+      </c>
+      <c r="M13" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="N13" s="0" t="s">
         <v>19</v>
       </c>
     </row>
@@ -2197,40 +2231,41 @@
       <c r="A14" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="B14" s="7" t="s">
-        <v>15</v>
-      </c>
+      <c r="B14" s="1"/>
       <c r="C14" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="D14" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="D14" s="7" t="n">
-        <v>0.0062</v>
-      </c>
-      <c r="E14" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="F14" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="G14" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="H14" s="11" t="s">
-        <v>17</v>
+      <c r="E14" s="7" t="n">
+        <v>0.0062</v>
+      </c>
+      <c r="F14" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="G14" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="H14" s="10" t="s">
+        <v>23</v>
       </c>
       <c r="I14" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="J14" s="2" t="s">
-        <v>18</v>
+      <c r="J14" s="11" t="s">
+        <v>17</v>
       </c>
       <c r="K14" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="L14" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="M14" s="0" t="s">
+      <c r="L14" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="M14" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="N14" s="0" t="s">
         <v>19</v>
       </c>
     </row>
@@ -2238,40 +2273,41 @@
       <c r="A15" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="B15" s="7" t="s">
-        <v>15</v>
-      </c>
+      <c r="B15" s="1"/>
       <c r="C15" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="D15" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="D15" s="7" t="n">
-        <v>0.0062</v>
-      </c>
-      <c r="E15" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="F15" s="10" t="s">
-        <v>23</v>
+      <c r="E15" s="7" t="n">
+        <v>0.0062</v>
+      </c>
+      <c r="F15" s="8" t="s">
+        <v>17</v>
       </c>
       <c r="G15" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="H15" s="11" t="s">
-        <v>17</v>
+      <c r="H15" s="10" t="s">
+        <v>23</v>
       </c>
       <c r="I15" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="J15" s="2" t="s">
-        <v>18</v>
+      <c r="J15" s="11" t="s">
+        <v>17</v>
       </c>
       <c r="K15" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="L15" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="M15" s="0" t="s">
+      <c r="L15" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="M15" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="N15" s="0" t="s">
         <v>19</v>
       </c>
     </row>
@@ -2279,40 +2315,43 @@
       <c r="A16" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="B16" s="7" t="s">
-        <v>15</v>
+      <c r="B16" s="1" t="s">
+        <v>21</v>
       </c>
       <c r="C16" s="7" t="s">
-        <v>65</v>
-      </c>
-      <c r="D16" s="7" t="n">
-        <v>0.0062</v>
-      </c>
-      <c r="E16" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="F16" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="G16" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="H16" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="I16" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="J16" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="K16" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="D16" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="E16" s="7" t="n">
+        <v>0.0062</v>
+      </c>
+      <c r="F16" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="G16" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="H16" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="I16" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="J16" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="K16" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="L16" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="L16" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="M16" s="0" t="s">
+      <c r="M16" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="N16" s="0" t="s">
         <v>19</v>
       </c>
     </row>
@@ -2320,40 +2359,43 @@
       <c r="A17" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="B17" s="7" t="s">
-        <v>15</v>
+      <c r="B17" s="1" t="s">
+        <v>24</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>66</v>
-      </c>
-      <c r="D17" s="7" t="n">
-        <v>0.0062</v>
-      </c>
-      <c r="E17" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="F17" s="10" t="s">
-        <v>23</v>
+        <v>15</v>
+      </c>
+      <c r="D17" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="E17" s="7" t="n">
+        <v>0.0062</v>
+      </c>
+      <c r="F17" s="8" t="s">
+        <v>17</v>
       </c>
       <c r="G17" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="H17" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="I17" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="J17" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="K17" s="14" t="s">
+      <c r="H17" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="I17" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="J17" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="K17" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="L17" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="L17" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="M17" s="0" t="s">
+      <c r="M17" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="N17" s="0" t="s">
         <v>19</v>
       </c>
     </row>
@@ -2361,40 +2403,43 @@
       <c r="A18" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="B18" s="7" t="s">
-        <v>15</v>
+      <c r="B18" s="1" t="s">
+        <v>37</v>
       </c>
       <c r="C18" s="7" t="s">
-        <v>67</v>
-      </c>
-      <c r="D18" s="7" t="n">
-        <v>0.0062</v>
-      </c>
-      <c r="E18" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="F18" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="G18" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="H18" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="D18" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="E18" s="7" t="n">
+        <v>0.0062</v>
+      </c>
+      <c r="F18" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="G18" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="H18" s="10" t="s">
         <v>23</v>
       </c>
       <c r="I18" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="J18" s="14" t="s">
-        <v>28</v>
+      <c r="J18" s="13" t="s">
+        <v>23</v>
       </c>
       <c r="K18" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="L18" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="M18" s="0" t="s">
+      <c r="L18" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="M18" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="N18" s="0" t="s">
         <v>19</v>
       </c>
     </row>
@@ -2402,40 +2447,43 @@
       <c r="A19" s="24" t="s">
         <v>58</v>
       </c>
-      <c r="B19" s="7" t="s">
-        <v>15</v>
+      <c r="B19" s="24" t="s">
+        <v>39</v>
       </c>
       <c r="C19" s="7" t="s">
-        <v>68</v>
-      </c>
-      <c r="D19" s="7" t="n">
-        <v>0.0062</v>
-      </c>
-      <c r="E19" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="F19" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="G19" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="H19" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="D19" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="E19" s="7" t="n">
+        <v>0.0062</v>
+      </c>
+      <c r="F19" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="G19" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="H19" s="10" t="s">
         <v>23</v>
       </c>
       <c r="I19" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="J19" s="15" t="s">
+      <c r="J19" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="K19" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="K19" s="18" t="s">
+      <c r="L19" s="18" t="s">
         <v>31</v>
       </c>
-      <c r="L19" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="M19" s="0" t="s">
+      <c r="M19" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="N19" s="0" t="s">
         <v>19</v>
       </c>
     </row>
@@ -2443,40 +2491,41 @@
       <c r="A20" s="24" t="s">
         <v>59</v>
       </c>
-      <c r="B20" s="7" t="s">
+      <c r="B20" s="24"/>
+      <c r="C20" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="C20" s="7" t="s">
+      <c r="D20" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="D20" s="7" t="n">
-        <v>0.0062</v>
-      </c>
-      <c r="E20" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="F20" s="8" t="s">
-        <v>17</v>
+      <c r="E20" s="7" t="n">
+        <v>0.0062</v>
+      </c>
+      <c r="F20" s="10" t="s">
+        <v>23</v>
       </c>
       <c r="G20" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="H20" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="I20" s="2" t="s">
-        <v>18</v>
+      <c r="H20" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="I20" s="11" t="s">
+        <v>17</v>
       </c>
       <c r="J20" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="K20" s="7" t="s">
+      <c r="K20" s="2" t="s">
         <v>18</v>
       </c>
       <c r="L20" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="M20" s="12" t="s">
+      <c r="M20" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="N20" s="12" t="s">
         <v>19</v>
       </c>
     </row>
@@ -2484,40 +2533,41 @@
       <c r="A21" s="25" t="s">
         <v>60</v>
       </c>
-      <c r="B21" s="7" t="s">
+      <c r="B21" s="25"/>
+      <c r="C21" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="C21" s="7" t="s">
+      <c r="D21" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="D21" s="7" t="n">
-        <v>0.0062</v>
-      </c>
-      <c r="E21" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="F21" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="G21" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="H21" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="I21" s="2" t="s">
-        <v>18</v>
+      <c r="E21" s="7" t="n">
+        <v>0.0062</v>
+      </c>
+      <c r="F21" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="G21" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="H21" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="I21" s="11" t="s">
+        <v>17</v>
       </c>
       <c r="J21" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="K21" s="7" t="s">
+      <c r="K21" s="2" t="s">
         <v>18</v>
       </c>
       <c r="L21" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="M21" s="12" t="s">
+      <c r="M21" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="N21" s="12" t="s">
         <v>19</v>
       </c>
     </row>
@@ -2525,40 +2575,41 @@
       <c r="A22" s="25" t="s">
         <v>61</v>
       </c>
-      <c r="B22" s="7" t="s">
+      <c r="B22" s="25"/>
+      <c r="C22" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="C22" s="7" t="s">
+      <c r="D22" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="D22" s="7" t="n">
-        <v>0.0062</v>
-      </c>
-      <c r="E22" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="F22" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="G22" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="H22" s="11" t="s">
-        <v>17</v>
+      <c r="E22" s="7" t="n">
+        <v>0.0062</v>
+      </c>
+      <c r="F22" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="G22" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="H22" s="10" t="s">
+        <v>23</v>
       </c>
       <c r="I22" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="J22" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="K22" s="7" t="s">
+      <c r="J22" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="K22" s="2" t="s">
         <v>18</v>
       </c>
       <c r="L22" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="M22" s="12" t="s">
+      <c r="M22" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="N22" s="12" t="s">
         <v>19</v>
       </c>
     </row>
@@ -2566,40 +2617,43 @@
       <c r="A23" s="26" t="s">
         <v>62</v>
       </c>
-      <c r="B23" s="7" t="s">
+      <c r="B23" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="C23" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="C23" s="7" t="s">
-        <v>65</v>
-      </c>
-      <c r="D23" s="7" t="n">
-        <v>0.0062</v>
-      </c>
-      <c r="E23" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="F23" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="G23" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="H23" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="I23" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="J23" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="K23" s="18" t="s">
+      <c r="D23" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="E23" s="7" t="n">
+        <v>0.0062</v>
+      </c>
+      <c r="F23" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="G23" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="H23" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="I23" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="J23" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="K23" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="L23" s="18" t="s">
         <v>31</v>
       </c>
-      <c r="L23" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="M23" s="12" t="s">
+      <c r="M23" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="N23" s="12" t="s">
         <v>19</v>
       </c>
     </row>
@@ -2607,40 +2661,43 @@
       <c r="A24" s="27" t="n">
         <v>23</v>
       </c>
-      <c r="B24" s="7" t="s">
+      <c r="B24" s="27" t="n">
+        <v>14</v>
+      </c>
+      <c r="C24" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="C24" s="7" t="s">
-        <v>67</v>
-      </c>
-      <c r="D24" s="7" t="n">
-        <v>0.0062</v>
-      </c>
-      <c r="E24" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="F24" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="G24" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="H24" s="13" t="s">
+      <c r="D24" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="E24" s="7" t="n">
+        <v>0.0062</v>
+      </c>
+      <c r="F24" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="G24" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="H24" s="10" t="s">
         <v>23</v>
       </c>
       <c r="I24" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="J24" s="14" t="s">
-        <v>28</v>
+      <c r="J24" s="13" t="s">
+        <v>23</v>
       </c>
       <c r="K24" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="L24" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="M24" s="12" t="s">
+      <c r="L24" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="M24" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="N24" s="12" t="s">
         <v>19</v>
       </c>
     </row>
@@ -2648,105 +2705,129 @@
       <c r="A25" s="27" t="n">
         <v>24</v>
       </c>
-      <c r="B25" s="7" t="s">
+      <c r="B25" s="27" t="n">
+        <v>15</v>
+      </c>
+      <c r="C25" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="C25" s="7" t="s">
-        <v>68</v>
-      </c>
-      <c r="D25" s="7" t="n">
-        <v>0.0062</v>
-      </c>
-      <c r="E25" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="F25" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="G25" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="H25" s="13" t="s">
+      <c r="D25" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="E25" s="7" t="n">
+        <v>0.0062</v>
+      </c>
+      <c r="F25" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="G25" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="H25" s="10" t="s">
         <v>23</v>
       </c>
       <c r="I25" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="J25" s="15" t="s">
+      <c r="J25" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="K25" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="K25" s="18" t="s">
+      <c r="L25" s="18" t="s">
         <v>31</v>
       </c>
-      <c r="L25" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="M25" s="12" t="s">
+      <c r="M25" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="N25" s="12" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="27"/>
+      <c r="B26" s="27"/>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="27"/>
+      <c r="B27" s="27"/>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="27"/>
+      <c r="B28" s="27"/>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="27"/>
+      <c r="B29" s="27"/>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="27"/>
+      <c r="B30" s="27"/>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="28"/>
+      <c r="B31" s="28"/>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="28"/>
+      <c r="B32" s="28"/>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="28"/>
+      <c r="B33" s="28"/>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="28"/>
+      <c r="B34" s="28"/>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="28"/>
+      <c r="B35" s="28"/>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="28"/>
+      <c r="B36" s="28"/>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="28"/>
+      <c r="B37" s="28"/>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="28"/>
+      <c r="B38" s="28"/>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="28"/>
+      <c r="B39" s="28"/>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="28"/>
+      <c r="B40" s="28"/>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="28"/>
+      <c r="B41" s="28"/>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="28"/>
+      <c r="B42" s="28"/>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="28"/>
+      <c r="B43" s="28"/>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="28"/>
+      <c r="B44" s="28"/>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="28"/>
+      <c r="B45" s="28"/>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="28"/>
+      <c r="B46" s="28"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>